<commit_message>
YARN/RM Lab: Doing the Math finished
</commit_message>
<xml_diff>
--- a/resources/tools/YARNCalcs.xlsx
+++ b/resources/tools/YARNCalcs.xlsx
@@ -613,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3934,8 +3934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4139,12 +4139,11 @@
         <v>24</v>
       </c>
       <c r="F12" s="15">
-        <f>F3/F2/2</f>
-        <v>10312.533333333333</v>
+        <v>12288</v>
       </c>
       <c r="G12" s="7">
         <f>F3/F12</f>
-        <v>48</v>
+        <v>40.283333333333331</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4163,7 +4162,7 @@
       </c>
       <c r="F13" s="15">
         <f>F12*0.8</f>
-        <v>8250.0266666666666</v>
+        <v>9830.4000000000015</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>22</v>
@@ -4208,8 +4207,7 @@
         <v>30</v>
       </c>
       <c r="F15" s="15">
-        <f>F3/F2</f>
-        <v>20625.066666666666</v>
+        <v>16384</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4219,7 +4217,7 @@
       </c>
       <c r="F16" s="15">
         <f>0.8*F15</f>
-        <v>16500.053333333333</v>
+        <v>13107.2</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4280,8 +4278,8 @@
         <v>38</v>
       </c>
       <c r="F23" s="15">
-        <f>F12*0.8</f>
-        <v>8250.0266666666666</v>
+        <f>F12</f>
+        <v>12288</v>
       </c>
     </row>
     <row r="24" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4290,8 +4288,8 @@
         <v>39</v>
       </c>
       <c r="F24" s="15">
-        <f>F15*0.8</f>
-        <v>16500.053333333333</v>
+        <f>F15</f>
+        <v>16384</v>
       </c>
     </row>
     <row r="25" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4301,7 +4299,7 @@
       </c>
       <c r="F25" s="7">
         <f t="shared" ref="F25:F26" si="0">PRODUCT(0.8,F23)</f>
-        <v>6600.021333333334</v>
+        <v>9830.4000000000015</v>
       </c>
     </row>
     <row r="26" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4311,7 +4309,7 @@
       </c>
       <c r="F26" s="7">
         <f t="shared" si="0"/>
-        <v>13200.042666666668</v>
+        <v>13107.2</v>
       </c>
     </row>
     <row r="27" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>